<commit_message>
Created workbench dir and established correlation between SG GDP & Employment
</commit_message>
<xml_diff>
--- a/data/Labour Force SG.xlsx
+++ b/data/Labour Force SG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22CD5AB-5C9D-4140-A82E-B2E56D28F5C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B34831-5B98-4008-8AD9-A439D9D24CA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="raw" sheetId="1" r:id="rId1"/>
     <sheet name="processed" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">processed!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -257,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -269,14 +272,25 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -319,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -806,7 +820,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1129,32 +1144,32 @@
       <selection activeCell="AS6" sqref="AS6:AZ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="68.3671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="AZ5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1312,7 +1327,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>56</v>
       </c>
@@ -1470,7 +1485,7 @@
         <v>3713.9</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>58</v>
       </c>
@@ -1628,7 +1643,7 @@
         <v>3574</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -1786,7 +1801,7 @@
         <v>139.9</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -1944,7 +1959,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -2102,42 +2117,42 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2152,31 +2167,31 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="13.1015625" customWidth="1"/>
     <col min="3" max="3" width="13.7890625" customWidth="1"/>
     <col min="4" max="4" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="164" t="s">
+      <c r="B1" s="165" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="164" t="s">
+      <c r="C1" s="165" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="164" t="s">
+      <c r="D1" s="165" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2190,7 +2205,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2204,7 +2219,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -2218,7 +2233,7 @@
         <v>94.6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -2232,7 +2247,7 @@
         <v>102.8</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2246,7 +2261,7 @@
         <v>106.9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -2261,6 +2276,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{7C6C2415-F52E-4254-B511-F9CBEFBCAD67}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added analysis and visualization for SG Overall Employment and Graduate Employment
</commit_message>
<xml_diff>
--- a/data/Labour Force SG.xlsx
+++ b/data/Labour Force SG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B34831-5B98-4008-8AD9-A439D9D24CA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4D6A7B-3021-46B4-B2F8-7810870B60BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">processed!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="75">
   <si>
     <t>Subject: Labour, Employment, Wages and Productivity</t>
   </si>
@@ -260,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -288,6 +299,12 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -333,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -824,6 +841,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1140,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AS6" sqref="AS6:AZ9"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AY7" sqref="AY7:AY9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2164,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4923C43A-4A2C-49E6-AE1B-982B39F71056}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2251,13 +2269,13 @@
       <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="166">
         <v>3657</v>
       </c>
       <c r="C6">
         <v>3550.1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="166">
         <v>106.9</v>
       </c>
     </row>
@@ -2265,18 +2283,33 @@
       <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="166">
         <v>3675.6</v>
       </c>
       <c r="C7">
         <v>3575.3</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="166">
         <v>100.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="166">
+        <v>3742.5</v>
+      </c>
+      <c r="C8">
+        <v>3631.7</v>
+      </c>
+      <c r="D8" s="166">
+        <v>110.8</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7C6C2415-F52E-4254-B511-F9CBEFBCAD67}"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>